<commit_message>
Build from JWN PC
</commit_message>
<xml_diff>
--- a/data/score_table.xlsx
+++ b/data/score_table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10119"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sblanche/Desktop/GitHub/website/docs/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fff675f9af20735c/Desktop/mywebsite/website/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1D7E9643-459F-0D41-81D3-1C879C692604}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="8_{1D7E9643-459F-0D41-81D3-1C879C692604}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{810E7345-0778-4290-ACC1-55273622CBFB}"/>
   <bookViews>
-    <workbookView xWindow="3360" yWindow="980" windowWidth="14480" windowHeight="16900" xr2:uid="{415608D0-703B-3644-9AA1-9DDDDB42A465}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{415608D0-703B-3644-9AA1-9DDDDB42A465}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -505,17 +505,17 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="40.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -532,7 +532,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -549,7 +549,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -566,7 +566,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
@@ -576,10 +576,10 @@
       <c r="C4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="1"/>
+      <c r="D4" s="2"/>
       <c r="E4" s="1"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
@@ -592,7 +592,7 @@
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
@@ -605,7 +605,7 @@
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>8</v>
       </c>

</xml_diff>